<commit_message>
Tabelas para o artigo
</commit_message>
<xml_diff>
--- a/artigo/tabela_medias_P1-P2A-P2B.xlsx
+++ b/artigo/tabela_medias_P1-P2A-P2B.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.andreotti\Desktop\python_Inegradora_II\artigo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB6FCD9-14D1-4B81-BB1F-F6923D7FF282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E7472C-D310-47CF-B544-AADBC92CFB35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="915" windowWidth="25455" windowHeight="13695" xr2:uid="{A52E17BB-C77D-4874-A8DE-02EE40024505}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A52E17BB-C77D-4874-A8DE-02EE40024505}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -486,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{478ED8D2-298B-4372-8CC8-05DB76A60AA9}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,11 +532,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-    </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>9</v>
@@ -570,6 +565,9 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -633,11 +631,6 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-    </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>9</v>
@@ -703,6 +696,9 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -798,11 +794,6 @@
         <v>50.9009</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-    </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>9</v>
@@ -868,6 +859,9 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
       <c r="B15" t="s">
         <v>15</v>
       </c>

</xml_diff>